<commit_message>
Code update on 22_June_01
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ParaBank_TestData.xlsx
+++ b/src/test/resources/TestData/ParaBank_TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTests" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenNewAccountTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -40,13 +41,25 @@
   </si>
   <si>
     <t>verifyUserLoginwithEmptyCredentials</t>
+  </si>
+  <si>
+    <t>Account_Type</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>CHECKING</t>
+  </si>
+  <si>
+    <t>SAVINGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +80,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -77,7 +98,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,23 +130,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,58 +430,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>12345</v>
+      </c>
+      <c r="C3" s="4">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
-        <v>12345</v>
-      </c>
-      <c r="C3" s="6">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>